<commit_message>
Updated schedule 2026 01. Manually replaced Rashi -> Minakshi
</commit_message>
<xml_diff>
--- a/schedule_2026_1.xlsx
+++ b/schedule_2026_1.xlsx
@@ -77,205 +77,205 @@
     <t xml:space="preserve">Dr. Rajat Gupta</t>
   </si>
   <si>
+    <t xml:space="preserve">Dr. Minakshi Mishra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03/01/2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dr. Amit Tripathi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04/01/2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05/01/2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dr. Ashok Kumar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dr. Ashish Gupta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06/01/2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07/01/2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08/01/2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09/01/2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10/01/2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11/01/2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12/01/2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13/01/2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14/01/2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15/01/2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16/01/2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17/01/2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dr. Kritika Prasad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18/01/2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19/01/2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20/01/2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21/01/2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22/01/2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23/01/2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24/01/2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25/01/2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26/01/2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27/01/2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28/01/2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29/01/2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30/01/2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31/01/2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doctor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No. of OTs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No. of Nights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not Available</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14-18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">doctor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ot_duty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">morning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">evening</t>
+  </si>
+  <si>
+    <t xml:space="preserve">night</t>
+  </si>
+  <si>
+    <t xml:space="preserve">working_days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total_shifts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(5, 'Mon', 'night')|(5, 'Mon', 'ot_duty')|(12, 'Mon', 'night')|(12, 'Mon', 'ot_duty')|(14, 'Wed', 'ot_duty')|(15, 'Thu', 'ot_duty')|(17, 'Sat', 'ot_duty')|(18, 'Sun', 'ot_duty')|(19, 'Mon', 'night')|(19, 'Mon', 'ot_duty')|(26, 'Mon', 'night')|(26, 'Mon', 'ot_duty')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(3, 'Sat', 'ot_duty')|(4, 'Sun', 'ot_duty')|(6, 'Tue', 'ot_duty')|(13, 'Tue', 'ot_duty')|(16, 'Fri', 'night')|(20, 'Tue', 'ot_duty')|(21, 'Wed', 'ot_duty')|(24, 'Sat', 'night')|(27, 'Tue', 'ot_duty')|(31, 'Sat', 'ot_duty')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(2, 'Fri', 'ot_duty')|(7, 'Wed', 'ot_duty')|(9, 'Fri', 'ot_duty')|(10, 'Sat', 'ot_duty')|(11, 'Sun', 'ot_duty')|(16, 'Fri', 'ot_duty')|(20, 'Tue', 'night')|(23, 'Fri', 'ot_duty')|(30, 'Fri', 'ot_duty')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1, 'Thu', 'night')|(1, 'Thu', 'ot_duty')|(8, 'Thu', 'night')|(8, 'Thu', 'ot_duty')|(22, 'Thu', 'night')|(22, 'Thu', 'ot_duty')|(24, 'Sat', 'ot_duty')|(25, 'Sun', 'ot_duty')|(28, 'Wed', 'ot_duty')|(29, 'Thu', 'night')|(29, 'Thu', 'ot_duty')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1, 'Thu', 'morning')|(3, 'Sat', 'morning')|(4, 'Sun', 'night')|(8, 'Thu', 'evening')|(9, 'Fri', 'morning')|(10, 'Sat', 'evening')|(11, 'Sun', 'night')|(18, 'Sun', 'night')|(20, 'Tue', 'evening')|(21, 'Wed', 'morning')|(22, 'Thu', 'evening')|(24, 'Sat', 'evening')|(25, 'Sun', 'night')|(28, 'Wed', 'morning')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(5, 'Mon', 'morning')|(6, 'Tue', 'morning')|(9, 'Fri', 'night')|(11, 'Sun', 'evening')|(11, 'Sun', 'morning')|(13, 'Tue', 'morning')|(15, 'Thu', 'evening')|(16, 'Fri', 'evening')|(21, 'Wed', 'night')|(23, 'Fri', 'night')|(26, 'Mon', 'evening')|(28, 'Wed', 'evening')|(29, 'Thu', 'morning')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(2, 'Fri', 'evening')|(3, 'Sat', 'evening')|(7, 'Wed', 'evening')|(9, 'Fri', 'evening')|(10, 'Sat', 'morning')|(14, 'Wed', 'night')|(16, 'Fri', 'morning')|(17, 'Sat', 'night')|(24, 'Sat', 'morning')|(27, 'Tue', 'evening')|(30, 'Fri', 'morning')|(31, 'Sat', 'morning')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(17, 'Sat', 'evening')|(18, 'Sun', 'evening')|(18, 'Sun', 'morning')|(19, 'Mon', 'morning')|(20, 'Tue', 'morning')|(21, 'Wed', 'evening')|(22, 'Thu', 'morning')|(23, 'Fri', 'evening')|(27, 'Tue', 'morning')|(28, 'Wed', 'night')|(30, 'Fri', 'night')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(2, 'Fri', 'morning')|(3, 'Sat', 'night')|(6, 'Tue', 'evening')|(7, 'Wed', 'night')|(12, 'Mon', 'morning')|(13, 'Tue', 'night')|(15, 'Thu', 'morning')|(25, 'Sun', 'evening')|(25, 'Sun', 'morning')|(26, 'Mon', 'morning')|(31, 'Sat', 'evening')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1, 'Thu', 'evening')|(4, 'Sun', 'morning')|(6, 'Tue', 'night')|(8, 'Thu', 'morning')|(10, 'Sat', 'night')|(12, 'Mon', 'evening')|(14, 'Wed', 'morning')|(17, 'Sat', 'morning')|(23, 'Fri', 'morning')|(29, 'Thu', 'evening')|(31, 'Sat', 'night')</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dr. Rashmi Sharma</t>
   </si>
   <si>
-    <t xml:space="preserve">03/01/2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dr. Amit Tripathi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">04/01/2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sun</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05/01/2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dr. Ashok Kumar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dr. Ashish Gupta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06/01/2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07/01/2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">08/01/2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09/01/2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10/01/2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11/01/2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12/01/2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13/01/2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14/01/2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15/01/2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16/01/2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17/01/2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dr. Kritika Prasad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18/01/2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19/01/2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20/01/2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21/01/2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22/01/2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23/01/2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24/01/2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25/01/2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26/01/2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27/01/2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28/01/2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29/01/2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30/01/2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31/01/2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Doctor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No. of OTs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No. of Nights</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not Available</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14-18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">doctor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ot_duty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">morning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">evening</t>
-  </si>
-  <si>
-    <t xml:space="preserve">night</t>
-  </si>
-  <si>
-    <t xml:space="preserve">working_days</t>
-  </si>
-  <si>
-    <t xml:space="preserve">total_shifts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(5, 'Mon', 'night')|(5, 'Mon', 'ot_duty')|(12, 'Mon', 'night')|(12, 'Mon', 'ot_duty')|(14, 'Wed', 'ot_duty')|(15, 'Thu', 'ot_duty')|(17, 'Sat', 'ot_duty')|(18, 'Sun', 'ot_duty')|(19, 'Mon', 'night')|(19, 'Mon', 'ot_duty')|(26, 'Mon', 'night')|(26, 'Mon', 'ot_duty')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(3, 'Sat', 'ot_duty')|(4, 'Sun', 'ot_duty')|(6, 'Tue', 'ot_duty')|(13, 'Tue', 'ot_duty')|(16, 'Fri', 'night')|(20, 'Tue', 'ot_duty')|(21, 'Wed', 'ot_duty')|(24, 'Sat', 'night')|(27, 'Tue', 'ot_duty')|(31, 'Sat', 'ot_duty')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(2, 'Fri', 'ot_duty')|(7, 'Wed', 'ot_duty')|(9, 'Fri', 'ot_duty')|(10, 'Sat', 'ot_duty')|(11, 'Sun', 'ot_duty')|(16, 'Fri', 'ot_duty')|(20, 'Tue', 'night')|(23, 'Fri', 'ot_duty')|(30, 'Fri', 'ot_duty')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1, 'Thu', 'night')|(1, 'Thu', 'ot_duty')|(8, 'Thu', 'night')|(8, 'Thu', 'ot_duty')|(22, 'Thu', 'night')|(22, 'Thu', 'ot_duty')|(24, 'Sat', 'ot_duty')|(25, 'Sun', 'ot_duty')|(28, 'Wed', 'ot_duty')|(29, 'Thu', 'night')|(29, 'Thu', 'ot_duty')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1, 'Thu', 'morning')|(3, 'Sat', 'morning')|(4, 'Sun', 'night')|(8, 'Thu', 'evening')|(9, 'Fri', 'morning')|(10, 'Sat', 'evening')|(11, 'Sun', 'night')|(18, 'Sun', 'night')|(20, 'Tue', 'evening')|(21, 'Wed', 'morning')|(22, 'Thu', 'evening')|(24, 'Sat', 'evening')|(25, 'Sun', 'night')|(28, 'Wed', 'morning')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(5, 'Mon', 'morning')|(6, 'Tue', 'morning')|(9, 'Fri', 'night')|(11, 'Sun', 'evening')|(11, 'Sun', 'morning')|(13, 'Tue', 'morning')|(15, 'Thu', 'evening')|(16, 'Fri', 'evening')|(21, 'Wed', 'night')|(23, 'Fri', 'night')|(26, 'Mon', 'evening')|(28, 'Wed', 'evening')|(29, 'Thu', 'morning')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(2, 'Fri', 'evening')|(3, 'Sat', 'evening')|(7, 'Wed', 'evening')|(9, 'Fri', 'evening')|(10, 'Sat', 'morning')|(14, 'Wed', 'night')|(16, 'Fri', 'morning')|(17, 'Sat', 'night')|(24, 'Sat', 'morning')|(27, 'Tue', 'evening')|(30, 'Fri', 'morning')|(31, 'Sat', 'morning')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(17, 'Sat', 'evening')|(18, 'Sun', 'evening')|(18, 'Sun', 'morning')|(19, 'Mon', 'morning')|(20, 'Tue', 'morning')|(21, 'Wed', 'evening')|(22, 'Thu', 'morning')|(23, 'Fri', 'evening')|(27, 'Tue', 'morning')|(28, 'Wed', 'night')|(30, 'Fri', 'night')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(2, 'Fri', 'morning')|(3, 'Sat', 'night')|(6, 'Tue', 'evening')|(7, 'Wed', 'night')|(12, 'Mon', 'morning')|(13, 'Tue', 'night')|(15, 'Thu', 'morning')|(25, 'Sun', 'evening')|(25, 'Sun', 'morning')|(26, 'Mon', 'morning')|(31, 'Sat', 'evening')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1, 'Thu', 'evening')|(4, 'Sun', 'morning')|(6, 'Tue', 'night')|(8, 'Thu', 'morning')|(10, 'Sat', 'night')|(12, 'Mon', 'evening')|(14, 'Wed', 'morning')|(17, 'Sat', 'morning')|(23, 'Fri', 'morning')|(29, 'Thu', 'evening')|(31, 'Sat', 'night')</t>
-  </si>
-  <si>
     <t xml:space="preserve">(2, 'Fri', 'night')|(4, 'Sun', 'evening')|(5, 'Mon', 'evening')|(7, 'Wed', 'morning')|(13, 'Tue', 'evening')|(14, 'Wed', 'evening')|(15, 'Thu', 'night')|(19, 'Mon', 'evening')|(27, 'Tue', 'night')|(30, 'Fri', 'evening')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dr. Minakshi Mishra</t>
   </si>
   <si>
     <t xml:space="preserve">Dr. Sunita Ojha</t>
@@ -400,36 +400,40 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -740,917 +744,917 @@
   </sheetPr>
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="17.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="17.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="D4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="4" t="s">
+      <c r="F5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="2" t="s">
+      <c r="E9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="2" t="s">
+      <c r="D10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="3" t="s">
+      <c r="E11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="4" t="s">
+      <c r="F12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G15" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G18" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G19" s="4" t="s">
+      <c r="F19" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G20" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" s="2" t="s">
+      <c r="E21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G21" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" s="5" t="s">
+      <c r="D22" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F22" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="G22" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" s="2" t="s">
+      <c r="E23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G23" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G24" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F25" s="3" t="s">
+      <c r="E25" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="G25" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F26" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G26" s="4" t="s">
+      <c r="F26" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E27" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F27" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="G27" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E28" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F28" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="G28" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29" s="5" t="s">
+      <c r="D29" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="F29" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="G29" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E30" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F30" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G30" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E31" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F31" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="G31" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E32" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F32" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G32" s="3" t="s">
+      <c r="G32" s="4" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E35" s="6" t="s">
+      <c r="E35" s="7" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B36" s="2" t="n">
+      <c r="B36" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="C36" s="2" t="n">
+      <c r="C36" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="E36" s="0" t="s">
+      <c r="E36" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F36" s="0" t="s">
+      <c r="F36" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B37" s="2" t="n">
+      <c r="B37" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="C37" s="2" t="n">
+      <c r="C37" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="E37" s="0" t="s">
+      <c r="E37" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F37" s="0" t="s">
+      <c r="F37" s="1" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C38" s="2" t="n">
+      <c r="C38" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="E38" s="0" t="s">
+      <c r="E38" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F38" s="0" t="s">
+      <c r="F38" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B39" s="2" t="n">
+      <c r="B39" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="C39" s="2" t="n">
+      <c r="C39" s="3" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B40" s="2" t="s">
+      <c r="A40" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C40" s="2" t="n">
+      <c r="C40" s="3" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C41" s="2" t="n">
+      <c r="C41" s="3" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C42" s="2" t="n">
+      <c r="C42" s="3" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C43" s="2" t="n">
+      <c r="C43" s="3" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C44" s="2" t="n">
+      <c r="C44" s="3" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B45" s="2" t="n">
+      <c r="B45" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="C45" s="2" t="n">
+      <c r="C45" s="3" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C46" s="2" t="n">
+      <c r="C46" s="3" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="6" t="s">
+      <c r="A47" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B47" s="6" t="n">
+      <c r="B47" s="7" t="n">
         <v>31</v>
       </c>
-      <c r="C47" s="6" t="n">
+      <c r="C47" s="7" t="n">
         <v>31</v>
       </c>
     </row>
@@ -1674,325 +1678,325 @@
   </sheetPr>
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="8" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="0" t="n">
+      <c r="C2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="1" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="0" t="n">
+      <c r="C3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="1" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="0" t="n">
+      <c r="C4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4" s="1" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="C5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="0" t="n">
+      <c r="C5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="F5" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5" s="1" t="n">
         <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" s="0" t="n">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="F6" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6" s="1" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" s="0" t="n">
+      <c r="B7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="F7" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7" s="1" t="n">
         <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" s="0" t="n">
+      <c r="B8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="F8" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="G8" s="1" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" s="0" t="n">
+      <c r="B9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="F9" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="G9" s="1" t="n">
         <v>11</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" s="0" t="n">
+      <c r="B10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="F10" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="G10" s="1" t="n">
         <v>11</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" s="0" t="n">
+      <c r="B11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="F11" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="G11" s="1" t="n">
         <v>11</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="E12" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="G12" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="B13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" s="0" t="n">
+      <c r="B13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" s="0" t="n">
+      <c r="B14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>